<commit_message>
kota kota se jawa barat
</commit_message>
<xml_diff>
--- a/kota-kota di indonesia.xlsx
+++ b/kota-kota di indonesia.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ORGANISASI\DORMITORY\TARBIYAH AKHWAT\MENTORING\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travlendar Database\data kota\Timeline-dan-document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="kota se indonesia" sheetId="3" r:id="rId1"/>
+    <sheet name="data  kota" sheetId="2" r:id="rId2"/>
+    <sheet name="kota se jawa barat" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
   <si>
     <t>&lt;link href='https://www.blogger.com/dyn-css/authorization.css?targetBlogID=7697872286098350133&amp;amp;zx=9c7cc169-5982-4b0f-aa02-c7881f75ecba' rel='stylesheet'/&gt;</t>
   </si>
@@ -322,6 +324,318 @@
   </si>
   <si>
     <t>Kota Sorong</t>
+  </si>
+  <si>
+    <t>Kota Banda Aceh</t>
+  </si>
+  <si>
+    <t>Kota Langsa</t>
+  </si>
+  <si>
+    <t>Kota Lhokseumawe</t>
+  </si>
+  <si>
+    <t>Kota Sabang</t>
+  </si>
+  <si>
+    <t>Kota Subulussalam</t>
+  </si>
+  <si>
+    <t>Kota Binjai</t>
+  </si>
+  <si>
+    <t>Kota Gunungsitoli</t>
+  </si>
+  <si>
+    <t>Kota Medan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Padangsidempuan</t>
+  </si>
+  <si>
+    <t>Kota Pematangsiantar</t>
+  </si>
+  <si>
+    <t>Kota Sibolga</t>
+  </si>
+  <si>
+    <t>Kota Tanjungbalai</t>
+  </si>
+  <si>
+    <t>Kota Tebing Tinggi</t>
+  </si>
+  <si>
+    <t>Kota Bukittinggi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Dumai</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Batam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Jambi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Lubuklinggau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bandar Lampung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Cilegon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bandung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Administrasi Jakarta Barat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Magelang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Batu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bima</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pontianak</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Banjarbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Balikpapan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Makassar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bau-Bau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bitung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Ambon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Ternate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Padang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pekanbaru</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tanjung Pinang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Sungai Penuh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pagar Alam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Metro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Serang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Banjar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Administrasi Jakarta Pusat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pekalongan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Blitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Mataram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Singkawang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Banjarmasin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bontang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Palopo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Kendari</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Kotamobagu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tidore Kepulauan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Padangpanjang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Palembang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tangerang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bekasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Administrasi Jakarta Selatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Salatiga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Kediri</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Samarinda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Parepare</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Manado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pariaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Prabumulih</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tangerang Selatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Bogor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Administrasi Jakarta Timur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Semarang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Madiun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tomohon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Payakumbuh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Cimahi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Administrasi Jakarta Utara</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Surakarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Malang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Sawahlunto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Cirebon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tegal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Mojokerto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Solok</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Depok</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Pasuruan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Sukabumi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Probolinggo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Tasikmalaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kota Surabaya</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Bogor</t>
+  </si>
+  <si>
+    <t>Ciamis</t>
+  </si>
+  <si>
+    <t>Cianjur</t>
+  </si>
+  <si>
+    <t>Cirebon</t>
+  </si>
+  <si>
+    <t>Garut</t>
+  </si>
+  <si>
+    <t>Indramayu</t>
+  </si>
+  <si>
+    <t>Karawang</t>
+  </si>
+  <si>
+    <t>Kuningan</t>
+  </si>
+  <si>
+    <t>Majalengka</t>
+  </si>
+  <si>
+    <t>Pangandaran</t>
+  </si>
+  <si>
+    <t>Purwakarta</t>
+  </si>
+  <si>
+    <t>Subang</t>
+  </si>
+  <si>
+    <t>Sukabumi</t>
+  </si>
+  <si>
+    <t>Sumedang</t>
+  </si>
+  <si>
+    <t>Tasikmalaya</t>
   </si>
 </sst>
 </file>
@@ -363,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
@@ -380,6 +694,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,10 +984,607 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:CU26"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" style="8" customWidth="1"/>
+    <col min="33" max="33" width="24.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="27" style="8" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" style="8" customWidth="1"/>
+    <col min="36" max="36" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="37.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="39.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="36.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="37.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="54" max="67" width="9.140625" style="8"/>
+    <col min="68" max="68" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="69" max="73" width="9.140625" style="8"/>
+    <col min="74" max="74" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="21.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="19" style="8" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.140625" style="8"/>
+    <col min="85" max="85" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9.140625" style="8"/>
+    <col min="89" max="89" width="12.140625" style="8" customWidth="1"/>
+    <col min="90" max="90" width="15.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="9.140625" style="8"/>
+    <col min="92" max="92" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="9.140625" style="8"/>
+    <col min="95" max="95" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="26.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.140625" style="8"/>
+    <col min="99" max="99" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="100" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:99" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AR2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AS2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AT2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU2" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AV2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="AW2" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AZ2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BA2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="BB2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="BF2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BJ2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BK2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BL2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="BM2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="BN2" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="BO2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BP2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="BQ2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="BT2" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="BU2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="BW2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BX2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="BY2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BZ2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="CB2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="CC2" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="CD2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="CG2" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="CH2" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="CI2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="CJ2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="CK2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="CM2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="CN2" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="CO2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CP2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="CQ2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="CR2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="CS2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="CT2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU2" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="CE8"/>
+      <c r="CF8"/>
+    </row>
+    <row r="9" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="CE9"/>
+      <c r="CF9"/>
+    </row>
+    <row r="10" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="CE10"/>
+      <c r="CF10"/>
+    </row>
+    <row r="11" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="AC11"/>
+      <c r="AD11"/>
+    </row>
+    <row r="12" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="BV12"/>
+      <c r="BW12"/>
+      <c r="CC12"/>
+      <c r="CD12"/>
+      <c r="CN12"/>
+      <c r="CO12"/>
+    </row>
+    <row r="13" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="BV13"/>
+      <c r="BW13"/>
+      <c r="CC13"/>
+      <c r="CE13"/>
+      <c r="CF13"/>
+      <c r="CN13"/>
+      <c r="CO13"/>
+      <c r="CR13"/>
+      <c r="CS13"/>
+      <c r="CT13"/>
+    </row>
+    <row r="14" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BR14"/>
+      <c r="BS14"/>
+      <c r="BV14"/>
+      <c r="BW14"/>
+      <c r="CC14"/>
+      <c r="CE14"/>
+      <c r="CF14"/>
+      <c r="CN14"/>
+      <c r="CO14"/>
+      <c r="CR14"/>
+      <c r="CS14"/>
+      <c r="CT14"/>
+    </row>
+    <row r="15" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AY15"/>
+      <c r="AZ15"/>
+      <c r="BA15"/>
+      <c r="BB15"/>
+      <c r="BK15"/>
+      <c r="BL15"/>
+      <c r="BR15"/>
+      <c r="BS15"/>
+      <c r="CN15"/>
+      <c r="CO15"/>
+    </row>
+    <row r="16" spans="2:99" x14ac:dyDescent="0.25">
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BK16"/>
+      <c r="BL16"/>
+      <c r="CN16"/>
+      <c r="CO16"/>
+    </row>
+    <row r="17" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BK17"/>
+      <c r="BL17"/>
+      <c r="CN17"/>
+      <c r="CO17"/>
+    </row>
+    <row r="18" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
+    </row>
+    <row r="19" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BK19"/>
+      <c r="BL19"/>
+    </row>
+    <row r="20" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+    </row>
+    <row r="21" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BK21"/>
+      <c r="BL21"/>
+    </row>
+    <row r="22" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
+    </row>
+    <row r="23" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="4:93" x14ac:dyDescent="0.25">
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:C203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G206" sqref="G206"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G205" sqref="G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,4 +2329,224 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" t="s">
+        <v>195</v>
+      </c>
+      <c r="L1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O1" t="s">
+        <v>199</v>
+      </c>
+      <c r="P1" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>201</v>
+      </c>
+      <c r="R1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>